<commit_message>
bubble CO2 tweak + RTD test
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1a_Gas_Cell_Calibration/Fityk_results.xlsx
+++ b/docs/Examples/Example1a_Gas_Cell_Calibration/Fityk_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\DiadFit_outer\docs\Examples\Example1a_Gas_Cell_Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\Box\Berkeley_new\DiadFit_outer\docs\Examples\Example1a_Gas_Cell_Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49BFDE9-151C-4B4D-8E1D-64BC613BCF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD06726-1106-4511-B7FF-EDE5AC4AD834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF1FF9BC-1B90-4EFB-8E6E-B9863C148F5B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF1FF9BC-1B90-4EFB-8E6E-B9863C148F5B}"/>
   </bookViews>
   <sheets>
     <sheet name="112820_FULL" sheetId="1" r:id="rId1"/>
@@ -7337,10 +7337,10 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H55" sqref="H55"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>